<commit_message>
Excel update & scores reading
</commit_message>
<xml_diff>
--- a/TopEducationApp/studentGrades.xlsx
+++ b/TopEducationApp/studentGrades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Cosas Progra\TINGESO\TINGESO-EV-01\TopEducationApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A512AEF3-E0BB-41C2-95F6-612BF99EBB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577FBE09-EBC9-4FAE-B3F7-C51D8F07479C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StudentList" sheetId="6" r:id="rId1"/>
@@ -3096,8 +3096,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3137,7 +3137,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>6.5</v>
+        <v>854</v>
       </c>
       <c r="D2" s="14">
         <v>44953</v>
@@ -3157,7 +3157,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="5">
-        <v>3.7</v>
+        <v>938</v>
       </c>
       <c r="D3" s="14">
         <v>44953</v>
@@ -3177,7 +3177,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>4.2</v>
+        <v>793</v>
       </c>
       <c r="D4" s="14">
         <v>44953</v>
@@ -3197,7 +3197,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="5">
-        <v>5.8</v>
+        <v>867</v>
       </c>
       <c r="D5" s="14">
         <v>44953</v>
@@ -3217,7 +3217,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="5">
-        <v>2.9</v>
+        <v>956</v>
       </c>
       <c r="D6" s="14">
         <v>44953</v>
@@ -3237,7 +3237,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="5">
-        <v>7</v>
+        <v>780</v>
       </c>
       <c r="D7" s="14">
         <v>44953</v>
@@ -3257,7 +3257,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="5">
-        <v>4.3</v>
+        <v>899</v>
       </c>
       <c r="D8" s="14">
         <v>44953</v>
@@ -3277,7 +3277,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="5">
-        <v>6.1</v>
+        <v>927</v>
       </c>
       <c r="D9" s="14">
         <v>44953</v>
@@ -3297,7 +3297,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="5">
-        <v>5.4</v>
+        <v>764</v>
       </c>
       <c r="D10" s="14">
         <v>44953</v>
@@ -3317,7 +3317,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="5">
-        <v>3.6</v>
+        <v>801</v>
       </c>
       <c r="D11" s="14">
         <v>44953</v>
@@ -3337,7 +3337,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="5">
-        <v>7</v>
+        <v>871</v>
       </c>
       <c r="D12" s="14">
         <v>44953</v>
@@ -3357,7 +3357,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="5">
-        <v>4.8</v>
+        <v>962</v>
       </c>
       <c r="D13" s="14">
         <v>44953</v>
@@ -3377,7 +3377,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="5">
-        <v>2.5</v>
+        <v>817</v>
       </c>
       <c r="D14" s="14">
         <v>44953</v>
@@ -3397,7 +3397,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="5">
-        <v>6.7</v>
+        <v>752</v>
       </c>
       <c r="D15" s="14">
         <v>44953</v>
@@ -3417,7 +3417,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="5">
-        <v>5.2</v>
+        <v>988</v>
       </c>
       <c r="D16" s="14">
         <v>44953</v>
@@ -3437,7 +3437,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="5">
-        <v>3.4</v>
+        <v>890</v>
       </c>
       <c r="D17" s="14">
         <v>44953</v>
@@ -3457,7 +3457,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="5">
-        <v>7</v>
+        <v>784</v>
       </c>
       <c r="D18" s="14">
         <v>44953</v>
@@ -3477,7 +3477,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="5">
-        <v>4.0999999999999996</v>
+        <v>943</v>
       </c>
       <c r="D19" s="14">
         <v>44953</v>
@@ -3497,7 +3497,7 @@
         <v>10</v>
       </c>
       <c r="C20" s="5">
-        <v>6.3</v>
+        <v>975</v>
       </c>
       <c r="D20" s="14">
         <v>44953</v>
@@ -3517,7 +3517,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="5">
-        <v>2.8</v>
+        <v>826</v>
       </c>
       <c r="D21" s="14">
         <v>44953</v>
@@ -3537,7 +3537,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="5">
-        <v>5.5</v>
+        <v>902</v>
       </c>
       <c r="D22" s="14">
         <v>44953</v>
@@ -3557,7 +3557,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="5">
-        <v>3.2</v>
+        <v>769</v>
       </c>
       <c r="D23" s="14">
         <v>44953</v>
@@ -3577,7 +3577,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="5">
-        <v>6.9</v>
+        <v>810</v>
       </c>
       <c r="D24" s="14">
         <v>44953</v>
@@ -3597,7 +3597,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="5">
-        <v>4.5999999999999996</v>
+        <v>976</v>
       </c>
       <c r="D25" s="14">
         <v>44953</v>
@@ -3617,7 +3617,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="5">
-        <v>2.7</v>
+        <v>955</v>
       </c>
       <c r="D26" s="14">
         <v>44953</v>
@@ -3637,7 +3637,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="5">
-        <v>7</v>
+        <v>791</v>
       </c>
       <c r="D27" s="14">
         <v>44953</v>
@@ -3657,7 +3657,7 @@
         <v>7</v>
       </c>
       <c r="C28" s="5">
-        <v>5.9</v>
+        <v>937</v>
       </c>
       <c r="D28" s="14">
         <v>44953</v>
@@ -3677,7 +3677,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="5">
-        <v>3.9</v>
+        <v>899</v>
       </c>
       <c r="D29" s="14">
         <v>44953</v>
@@ -3697,7 +3697,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="5">
-        <v>6.2</v>
+        <v>768</v>
       </c>
       <c r="D30" s="14">
         <v>44953</v>
@@ -3717,7 +3717,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="7">
-        <v>4.5</v>
+        <v>834</v>
       </c>
       <c r="D31" s="16">
         <v>44953</v>
@@ -3744,7 +3744,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3783,7 +3783,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>5.6</v>
+        <v>802</v>
       </c>
       <c r="D2" s="14">
         <v>44981</v>
@@ -3803,7 +3803,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="5">
-        <v>3.9</v>
+        <v>967</v>
       </c>
       <c r="D3" s="14">
         <v>44981</v>
@@ -3823,7 +3823,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>6.4</v>
+        <v>754</v>
       </c>
       <c r="D4" s="14">
         <v>44981</v>
@@ -3843,7 +3843,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="5">
-        <v>4.7</v>
+        <v>893</v>
       </c>
       <c r="D5" s="14">
         <v>44981</v>
@@ -3863,7 +3863,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="5">
-        <v>2.8</v>
+        <v>817</v>
       </c>
       <c r="D6" s="14">
         <v>44981</v>
@@ -3883,7 +3883,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="5">
-        <v>6.1</v>
+        <v>981</v>
       </c>
       <c r="D7" s="14">
         <v>44981</v>
@@ -3903,7 +3903,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="5">
-        <v>5.2</v>
+        <v>770</v>
       </c>
       <c r="D8" s="14">
         <v>44981</v>
@@ -3923,7 +3923,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="5">
-        <v>4.9000000000000004</v>
+        <v>868</v>
       </c>
       <c r="D9" s="14">
         <v>44981</v>
@@ -3943,7 +3943,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="5">
-        <v>3.3</v>
+        <v>799</v>
       </c>
       <c r="D10" s="14">
         <v>44981</v>
@@ -3963,7 +3963,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="5">
-        <v>7</v>
+        <v>945</v>
       </c>
       <c r="D11" s="14">
         <v>44981</v>
@@ -3983,7 +3983,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="5">
-        <v>4.5</v>
+        <v>764</v>
       </c>
       <c r="D12" s="14">
         <v>44981</v>
@@ -4003,7 +4003,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="5">
-        <v>6.7</v>
+        <v>956</v>
       </c>
       <c r="D13" s="14">
         <v>44981</v>
@@ -4023,7 +4023,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="5">
-        <v>3.8</v>
+        <v>791</v>
       </c>
       <c r="D14" s="14">
         <v>44981</v>
@@ -4043,7 +4043,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="5">
-        <v>5.3</v>
+        <v>823</v>
       </c>
       <c r="D15" s="14">
         <v>44981</v>
@@ -4063,7 +4063,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="5">
-        <v>2.6</v>
+        <v>982</v>
       </c>
       <c r="D16" s="14">
         <v>44981</v>
@@ -4083,7 +4083,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="5">
-        <v>6</v>
+        <v>871</v>
       </c>
       <c r="D17" s="14">
         <v>44981</v>
@@ -4103,7 +4103,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="5">
-        <v>4.2</v>
+        <v>898</v>
       </c>
       <c r="D18" s="14">
         <v>44981</v>
@@ -4123,7 +4123,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="5">
-        <v>7</v>
+        <v>938</v>
       </c>
       <c r="D19" s="14">
         <v>44981</v>
@@ -4143,7 +4143,7 @@
         <v>10</v>
       </c>
       <c r="C20" s="5">
-        <v>5.0999999999999996</v>
+        <v>789</v>
       </c>
       <c r="D20" s="14">
         <v>44981</v>
@@ -4163,7 +4163,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="5">
-        <v>3.7</v>
+        <v>903</v>
       </c>
       <c r="D21" s="14">
         <v>44981</v>
@@ -4183,7 +4183,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="5">
-        <v>6.5</v>
+        <v>785</v>
       </c>
       <c r="D22" s="14">
         <v>44981</v>
@@ -4203,7 +4203,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="5">
-        <v>4.8</v>
+        <v>972</v>
       </c>
       <c r="D23" s="14">
         <v>44981</v>
@@ -4223,7 +4223,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="5">
-        <v>2.9</v>
+        <v>752</v>
       </c>
       <c r="D24" s="14">
         <v>44981</v>
@@ -4243,7 +4243,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="5">
-        <v>5.4</v>
+        <v>965</v>
       </c>
       <c r="D25" s="14">
         <v>44981</v>
@@ -4263,7 +4263,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="5">
-        <v>3.6</v>
+        <v>809</v>
       </c>
       <c r="D26" s="14">
         <v>44981</v>
@@ -4283,7 +4283,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="5">
-        <v>7</v>
+        <v>920</v>
       </c>
       <c r="D27" s="14">
         <v>44981</v>
@@ -4303,7 +4303,7 @@
         <v>7</v>
       </c>
       <c r="C28" s="5">
-        <v>6.2</v>
+        <v>785</v>
       </c>
       <c r="D28" s="14">
         <v>44981</v>
@@ -4323,7 +4323,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="5">
-        <v>4.3</v>
+        <v>952</v>
       </c>
       <c r="D29" s="14">
         <v>44981</v>
@@ -4343,7 +4343,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="5">
-        <v>2.7</v>
+        <v>976</v>
       </c>
       <c r="D30" s="14">
         <v>44981</v>
@@ -4363,7 +4363,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="7">
-        <v>5.9</v>
+        <v>793</v>
       </c>
       <c r="D31" s="16">
         <v>44981</v>
@@ -4389,7 +4389,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C31" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4428,7 +4428,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>4.8</v>
+        <v>862</v>
       </c>
       <c r="D2" s="14">
         <v>45016</v>
@@ -4448,7 +4448,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="5">
-        <v>3.3</v>
+        <v>787</v>
       </c>
       <c r="D3" s="14">
         <v>45016</v>
@@ -4468,7 +4468,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>5.6</v>
+        <v>925</v>
       </c>
       <c r="D4" s="14">
         <v>45016</v>
@@ -4488,7 +4488,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="5">
-        <v>6.4</v>
+        <v>978</v>
       </c>
       <c r="D5" s="14">
         <v>45016</v>
@@ -4508,7 +4508,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="5">
-        <v>2.7</v>
+        <v>801</v>
       </c>
       <c r="D6" s="14">
         <v>45016</v>
@@ -4528,7 +4528,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="5">
-        <v>5.0999999999999996</v>
+        <v>954</v>
       </c>
       <c r="D7" s="14">
         <v>45016</v>
@@ -4548,7 +4548,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="5">
-        <v>4.2</v>
+        <v>769</v>
       </c>
       <c r="D8" s="14">
         <v>45016</v>
@@ -4568,7 +4568,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="5">
-        <v>6</v>
+        <v>840</v>
       </c>
       <c r="D9" s="14">
         <v>45016</v>
@@ -4588,7 +4588,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="5">
-        <v>3.7</v>
+        <v>892</v>
       </c>
       <c r="D10" s="14">
         <v>45016</v>
@@ -4608,7 +4608,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="5">
-        <v>4.9000000000000004</v>
+        <v>759</v>
       </c>
       <c r="D11" s="14">
         <v>45016</v>
@@ -4628,7 +4628,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="5">
-        <v>6.5</v>
+        <v>983</v>
       </c>
       <c r="D12" s="14">
         <v>45016</v>
@@ -4648,7 +4648,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="5">
-        <v>5.2</v>
+        <v>872</v>
       </c>
       <c r="D13" s="14">
         <v>45016</v>
@@ -4668,7 +4668,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="5">
-        <v>2.8</v>
+        <v>937</v>
       </c>
       <c r="D14" s="14">
         <v>45016</v>
@@ -4688,7 +4688,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="5">
-        <v>3.9</v>
+        <v>794</v>
       </c>
       <c r="D15" s="14">
         <v>45016</v>
@@ -4708,7 +4708,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="5">
-        <v>7</v>
+        <v>968</v>
       </c>
       <c r="D16" s="14">
         <v>45016</v>
@@ -4728,7 +4728,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="5">
-        <v>4.3</v>
+        <v>783</v>
       </c>
       <c r="D17" s="14">
         <v>45016</v>
@@ -4748,7 +4748,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="5">
-        <v>6.1</v>
+        <v>965</v>
       </c>
       <c r="D18" s="14">
         <v>45016</v>
@@ -4768,7 +4768,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="5">
-        <v>5.4</v>
+        <v>812</v>
       </c>
       <c r="D19" s="14">
         <v>45016</v>
@@ -4788,7 +4788,7 @@
         <v>10</v>
       </c>
       <c r="C20" s="5">
-        <v>2.6</v>
+        <v>911</v>
       </c>
       <c r="D20" s="14">
         <v>45016</v>
@@ -4808,7 +4808,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="5">
-        <v>4.7</v>
+        <v>758</v>
       </c>
       <c r="D21" s="14">
         <v>45016</v>
@@ -4828,7 +4828,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="5">
-        <v>3.6</v>
+        <v>991</v>
       </c>
       <c r="D22" s="14">
         <v>45016</v>
@@ -4848,7 +4848,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="5">
-        <v>5.9</v>
+        <v>902</v>
       </c>
       <c r="D23" s="14">
         <v>45016</v>
@@ -4868,7 +4868,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="5">
-        <v>7</v>
+        <v>782</v>
       </c>
       <c r="D24" s="14">
         <v>45016</v>
@@ -4888,7 +4888,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="5">
-        <v>4.5</v>
+        <v>959</v>
       </c>
       <c r="D25" s="14">
         <v>45016</v>
@@ -4908,7 +4908,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="5">
-        <v>6.7</v>
+        <v>827</v>
       </c>
       <c r="D26" s="14">
         <v>45016</v>
@@ -4928,7 +4928,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="5">
-        <v>3.8</v>
+        <v>903</v>
       </c>
       <c r="D27" s="14">
         <v>45016</v>
@@ -4948,7 +4948,7 @@
         <v>7</v>
       </c>
       <c r="C28" s="5">
-        <v>5.3</v>
+        <v>773</v>
       </c>
       <c r="D28" s="14">
         <v>45016</v>
@@ -4968,7 +4968,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="5">
-        <v>2.9</v>
+        <v>898</v>
       </c>
       <c r="D29" s="14">
         <v>45016</v>
@@ -4988,7 +4988,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="5">
-        <v>4.2</v>
+        <v>965</v>
       </c>
       <c r="D30" s="14">
         <v>45016</v>
@@ -5008,7 +5008,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="7">
-        <v>6.3</v>
+        <v>789</v>
       </c>
       <c r="D31" s="16">
         <v>45016</v>
@@ -5034,7 +5034,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5073,7 +5073,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>5.4</v>
+        <v>972</v>
       </c>
       <c r="D2" s="14">
         <v>45044</v>
@@ -5093,7 +5093,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="5">
-        <v>4.8</v>
+        <v>794</v>
       </c>
       <c r="D3" s="14">
         <v>45044</v>
@@ -5113,7 +5113,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>6.2</v>
+        <v>812</v>
       </c>
       <c r="D4" s="14">
         <v>45044</v>
@@ -5133,7 +5133,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="5">
-        <v>3.7</v>
+        <v>965</v>
       </c>
       <c r="D5" s="14">
         <v>45044</v>
@@ -5153,7 +5153,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="5">
-        <v>7</v>
+        <v>889</v>
       </c>
       <c r="D6" s="14">
         <v>45044</v>
@@ -5173,7 +5173,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="5">
-        <v>4.5999999999999996</v>
+        <v>769</v>
       </c>
       <c r="D7" s="14">
         <v>45044</v>
@@ -5193,7 +5193,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="5">
-        <v>5.9</v>
+        <v>825</v>
       </c>
       <c r="D8" s="14">
         <v>45044</v>
@@ -5213,7 +5213,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="5">
-        <v>3.2</v>
+        <v>782</v>
       </c>
       <c r="D9" s="14">
         <v>45044</v>
@@ -5233,7 +5233,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="5">
-        <v>6.5</v>
+        <v>938</v>
       </c>
       <c r="D10" s="14">
         <v>45044</v>
@@ -5253,7 +5253,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="5">
-        <v>2.9</v>
+        <v>851</v>
       </c>
       <c r="D11" s="14">
         <v>45044</v>
@@ -5273,7 +5273,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="5">
-        <v>4.4000000000000004</v>
+        <v>797</v>
       </c>
       <c r="D12" s="14">
         <v>45044</v>
@@ -5293,7 +5293,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="5">
-        <v>7</v>
+        <v>902</v>
       </c>
       <c r="D13" s="14">
         <v>45044</v>
@@ -5313,7 +5313,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="5">
-        <v>5.0999999999999996</v>
+        <v>763</v>
       </c>
       <c r="D14" s="14">
         <v>45044</v>
@@ -5333,7 +5333,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="5">
-        <v>3.6</v>
+        <v>983</v>
       </c>
       <c r="D15" s="14">
         <v>45044</v>
@@ -5353,7 +5353,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="5">
-        <v>6.3</v>
+        <v>860</v>
       </c>
       <c r="D16" s="14">
         <v>45044</v>
@@ -5373,7 +5373,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="5">
-        <v>4.5</v>
+        <v>775</v>
       </c>
       <c r="D17" s="14">
         <v>45044</v>
@@ -5393,7 +5393,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="5">
-        <v>2.7</v>
+        <v>956</v>
       </c>
       <c r="D18" s="14">
         <v>45044</v>
@@ -5413,7 +5413,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="5">
-        <v>5.8</v>
+        <v>791</v>
       </c>
       <c r="D19" s="14">
         <v>45044</v>
@@ -5433,7 +5433,7 @@
         <v>10</v>
       </c>
       <c r="C20" s="5">
-        <v>3.4</v>
+        <v>872</v>
       </c>
       <c r="D20" s="14">
         <v>45044</v>
@@ -5453,7 +5453,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="5">
-        <v>7</v>
+        <v>928</v>
       </c>
       <c r="D21" s="14">
         <v>45044</v>
@@ -5473,7 +5473,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="5">
-        <v>6.1</v>
+        <v>810</v>
       </c>
       <c r="D22" s="14">
         <v>45044</v>
@@ -5493,7 +5493,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="5">
-        <v>4.2</v>
+        <v>759</v>
       </c>
       <c r="D23" s="14">
         <v>45044</v>
@@ -5513,7 +5513,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="5">
-        <v>2.8</v>
+        <v>967</v>
       </c>
       <c r="D24" s="14">
         <v>45044</v>
@@ -5533,7 +5533,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="5">
-        <v>5.6</v>
+        <v>925</v>
       </c>
       <c r="D25" s="14">
         <v>45044</v>
@@ -5553,7 +5553,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="5">
-        <v>3.3</v>
+        <v>788</v>
       </c>
       <c r="D26" s="14">
         <v>45044</v>
@@ -5573,7 +5573,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="5">
-        <v>6.4</v>
+        <v>942</v>
       </c>
       <c r="D27" s="14">
         <v>45044</v>
@@ -5593,7 +5593,7 @@
         <v>7</v>
       </c>
       <c r="C28" s="5">
-        <v>2.5</v>
+        <v>869</v>
       </c>
       <c r="D28" s="14">
         <v>45044</v>
@@ -5613,7 +5613,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="5">
-        <v>4.9000000000000004</v>
+        <v>976</v>
       </c>
       <c r="D29" s="14">
         <v>45044</v>
@@ -5633,7 +5633,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="5">
-        <v>7</v>
+        <v>791</v>
       </c>
       <c r="D30" s="14">
         <v>45044</v>
@@ -5653,7 +5653,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="7">
-        <v>5.7</v>
+        <v>832</v>
       </c>
       <c r="D31" s="16">
         <v>45044</v>
@@ -5676,10 +5676,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E35A56-AEC5-4A26-8115-B1037363C57C}">
   <sheetPr codeName="Hoja5"/>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5718,7 +5718,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>5.2</v>
+        <v>893</v>
       </c>
       <c r="D2" s="14">
         <v>45072</v>
@@ -5738,7 +5738,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="5">
-        <v>6.3</v>
+        <v>817</v>
       </c>
       <c r="D3" s="14">
         <v>45072</v>
@@ -5758,7 +5758,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>4.7</v>
+        <v>964</v>
       </c>
       <c r="D4" s="14">
         <v>45072</v>
@@ -5778,7 +5778,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="5">
-        <v>3.9</v>
+        <v>782</v>
       </c>
       <c r="D5" s="14">
         <v>45072</v>
@@ -5798,7 +5798,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="5">
-        <v>6.1</v>
+        <v>926</v>
       </c>
       <c r="D6" s="14">
         <v>45072</v>
@@ -5818,7 +5818,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="5">
-        <v>4.5</v>
+        <v>798</v>
       </c>
       <c r="D7" s="14">
         <v>45072</v>
@@ -5838,7 +5838,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="5">
-        <v>5.8</v>
+        <v>952</v>
       </c>
       <c r="D8" s="14">
         <v>45072</v>
@@ -5858,7 +5858,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="5">
-        <v>3.6</v>
+        <v>867</v>
       </c>
       <c r="D9" s="14">
         <v>45072</v>
@@ -5878,7 +5878,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="5">
-        <v>2.8</v>
+        <v>791</v>
       </c>
       <c r="D10" s="14">
         <v>45072</v>
@@ -5898,7 +5898,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="5">
-        <v>6.4</v>
+        <v>811</v>
       </c>
       <c r="D11" s="14">
         <v>45072</v>
@@ -5918,7 +5918,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="5">
-        <v>4.9000000000000004</v>
+        <v>975</v>
       </c>
       <c r="D12" s="14">
         <v>45072</v>
@@ -5938,7 +5938,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="5">
-        <v>3.5</v>
+        <v>757</v>
       </c>
       <c r="D13" s="14">
         <v>45072</v>
@@ -5958,7 +5958,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="5">
-        <v>5.7</v>
+        <v>938</v>
       </c>
       <c r="D14" s="14">
         <v>45072</v>
@@ -5978,7 +5978,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="5">
-        <v>7</v>
+        <v>859</v>
       </c>
       <c r="D15" s="14">
         <v>45072</v>
@@ -5998,7 +5998,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="5">
-        <v>4.2</v>
+        <v>790</v>
       </c>
       <c r="D16" s="14">
         <v>45072</v>
@@ -6010,7 +6010,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="5">
-        <v>6</v>
+        <v>928</v>
       </c>
       <c r="D17" s="14">
         <v>45072</v>
@@ -6030,7 +6030,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="5">
-        <v>2.7</v>
+        <v>805</v>
       </c>
       <c r="D18" s="14">
         <v>45072</v>
@@ -6050,7 +6050,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="5">
-        <v>5.4</v>
+        <v>863</v>
       </c>
       <c r="D19" s="14">
         <v>45072</v>
@@ -6070,7 +6070,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>10</v>
       </c>
       <c r="C20" s="5">
-        <v>3.8</v>
+        <v>786</v>
       </c>
       <c r="D20" s="14">
         <v>45072</v>
@@ -6090,7 +6090,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="5">
-        <v>6.2</v>
+        <v>976</v>
       </c>
       <c r="D21" s="14">
         <v>45072</v>
@@ -6110,7 +6110,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="5">
-        <v>4.5999999999999996</v>
+        <v>899</v>
       </c>
       <c r="D22" s="14">
         <v>45072</v>
@@ -6130,7 +6130,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="5">
-        <v>5.0999999999999996</v>
+        <v>764</v>
       </c>
       <c r="D23" s="14">
         <v>45072</v>
@@ -6150,7 +6150,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="5">
-        <v>3.7</v>
+        <v>931</v>
       </c>
       <c r="D24" s="14">
         <v>45072</v>
@@ -6169,8 +6169,9 @@
       <c r="F24" s="15" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L24" s="18"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -6178,7 +6179,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="5">
-        <v>2.9</v>
+        <v>843</v>
       </c>
       <c r="D25" s="14">
         <v>45072</v>
@@ -6190,7 +6191,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -6198,7 +6199,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="5">
-        <v>5.6</v>
+        <v>972</v>
       </c>
       <c r="D26" s="14">
         <v>45072</v>
@@ -6210,7 +6211,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -6218,7 +6219,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="5">
-        <v>4.4000000000000004</v>
+        <v>816</v>
       </c>
       <c r="D27" s="14">
         <v>45072</v>
@@ -6230,7 +6231,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -6238,7 +6239,7 @@
         <v>7</v>
       </c>
       <c r="C28" s="5">
-        <v>6.5</v>
+        <v>756</v>
       </c>
       <c r="D28" s="14">
         <v>45072</v>
@@ -6250,7 +6251,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -6258,7 +6259,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="5">
-        <v>7</v>
+        <v>915</v>
       </c>
       <c r="D29" s="14">
         <v>45072</v>
@@ -6270,7 +6271,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -6278,7 +6279,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="5">
-        <v>3.3</v>
+        <v>783</v>
       </c>
       <c r="D30" s="14">
         <v>45072</v>
@@ -6290,7 +6291,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -6298,7 +6299,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="7">
-        <v>4.9000000000000004</v>
+        <v>894</v>
       </c>
       <c r="D31" s="16">
         <v>45072</v>
@@ -6312,8 +6313,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implementation of average grade
</commit_message>
<xml_diff>
--- a/TopEducationApp/studentGrades.xlsx
+++ b/TopEducationApp/studentGrades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Cosas Progra\TINGESO\TINGESO-EV-01\TopEducationApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577FBE09-EBC9-4FAE-B3F7-C51D8F07479C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9F8772-61FF-4281-AB2B-209FD15DFE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="130">
   <si>
     <t>StudentID</t>
   </si>
@@ -74,12 +74,6 @@
     <t>21098765-4</t>
   </si>
   <si>
-    <t>67890123-2</t>
-  </si>
-  <si>
-    <t>45678901-1</t>
-  </si>
-  <si>
     <t>Score</t>
   </si>
   <si>
@@ -372,6 +366,60 @@
   </si>
   <si>
     <t>Birthdate</t>
+  </si>
+  <si>
+    <t>45678901-2</t>
+  </si>
+  <si>
+    <t>67890123-4</t>
+  </si>
+  <si>
+    <t>90123456-7</t>
+  </si>
+  <si>
+    <t>76543210-9</t>
+  </si>
+  <si>
+    <t>32109876-5</t>
+  </si>
+  <si>
+    <t>10987654-3</t>
+  </si>
+  <si>
+    <t>9876543-2</t>
+  </si>
+  <si>
+    <t>8765432-1</t>
+  </si>
+  <si>
+    <t>7654321-0</t>
+  </si>
+  <si>
+    <t>6543210-9</t>
+  </si>
+  <si>
+    <t>5432109-8</t>
+  </si>
+  <si>
+    <t>4321098-7</t>
+  </si>
+  <si>
+    <t>3210987-6</t>
+  </si>
+  <si>
+    <t>2109876-5</t>
+  </si>
+  <si>
+    <t>1098765-4</t>
+  </si>
+  <si>
+    <t>987654-3</t>
+  </si>
+  <si>
+    <t>876543-2</t>
+  </si>
+  <si>
+    <t>765432-1</t>
   </si>
 </sst>
 </file>
@@ -2259,7 +2307,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B2" sqref="B2:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,45 +2330,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" s="14">
         <v>33131</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H2" s="15">
         <v>2012</v>
@@ -2331,22 +2379,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" s="14">
         <v>35041</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H3" s="15">
         <v>2019</v>
@@ -2357,22 +2405,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" s="14">
         <v>35996</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H4" s="15">
         <v>2023</v>
@@ -2383,22 +2431,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5" s="14">
         <v>34403</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H5" s="15">
         <v>2021</v>
@@ -2409,22 +2457,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E6" s="14">
         <v>35737</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H6" s="15">
         <v>2018</v>
@@ -2435,22 +2483,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E7" s="14">
         <v>33751</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H7" s="15">
         <v>2013</v>
@@ -2461,22 +2509,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="14">
         <v>35234</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H8" s="15">
         <v>2023</v>
@@ -2487,22 +2535,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9" s="14">
         <v>34216</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H9" s="15">
         <v>2013</v>
@@ -2513,22 +2561,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E10" s="14">
         <v>33350</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H10" s="15">
         <v>2017</v>
@@ -2539,22 +2587,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E11" s="14">
         <v>36442</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H11" s="15">
         <v>2012</v>
@@ -2565,22 +2613,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E12" s="14">
         <v>32918</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H12" s="15">
         <v>2020</v>
@@ -2591,22 +2639,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" s="14">
         <v>34333</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H13" s="15">
         <v>2015</v>
@@ -2617,22 +2665,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E14" s="14">
         <v>34918</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H14" s="15">
         <v>1999</v>
@@ -2643,22 +2691,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E15" s="14">
         <v>35811</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H15" s="15">
         <v>2021</v>
@@ -2669,22 +2717,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" s="14">
         <v>33902</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H16" s="15">
         <v>2012</v>
@@ -2695,22 +2743,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E17" s="14">
         <v>34496</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H17" s="15">
         <v>2015</v>
@@ -2721,22 +2769,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E18" s="14">
         <v>35491</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H18" s="15">
         <v>2014</v>
@@ -2747,22 +2795,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E19" s="14">
         <v>33438</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H19" s="15">
         <v>2016</v>
@@ -2773,22 +2821,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E20" s="14">
         <v>33144</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H20" s="15">
         <v>2011</v>
@@ -2799,22 +2847,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E21" s="14">
         <v>35197</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H21" s="15">
         <v>2017</v>
@@ -2825,22 +2873,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" s="14">
         <v>36487</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H22" s="15">
         <v>2014</v>
@@ -2851,22 +2899,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E23" s="14">
         <v>33700</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H23" s="15">
         <v>2016</v>
@@ -2877,22 +2925,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E24" s="14">
         <v>34182</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H24" s="15">
         <v>2020</v>
@@ -2903,22 +2951,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E25" s="14">
         <v>34681</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H25" s="15">
         <v>2013</v>
@@ -2929,22 +2977,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E26" s="14">
         <v>35720</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H26" s="15">
         <v>2015</v>
@@ -2955,22 +3003,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E27" s="14">
         <v>35883</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H27" s="15">
         <v>2017</v>
@@ -2981,22 +3029,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E28" s="14">
         <v>33424</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H28" s="15">
         <v>2023</v>
@@ -3007,22 +3055,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>3</v>
+        <v>127</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E29" s="14">
         <v>33137</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H29" s="15">
         <v>2022</v>
@@ -3033,22 +3081,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E30" s="14">
         <v>34738</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H30" s="15">
         <v>2014</v>
@@ -3059,22 +3107,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E31" s="16">
         <v>35240</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H31" s="17">
         <v>2013</v>
@@ -3097,7 +3145,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C31"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,16 +3165,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3137,16 +3185,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>854</v>
+        <v>800</v>
       </c>
       <c r="D2" s="14">
         <v>44953</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3154,7 +3202,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5">
         <v>938</v>
@@ -3163,10 +3211,10 @@
         <v>44953</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3174,7 +3222,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5">
         <v>793</v>
@@ -3183,10 +3231,10 @@
         <v>44953</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3194,7 +3242,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="C5" s="5">
         <v>867</v>
@@ -3203,10 +3251,10 @@
         <v>44953</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3214,7 +3262,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5">
         <v>956</v>
@@ -3223,10 +3271,10 @@
         <v>44953</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3234,7 +3282,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="C7" s="5">
         <v>780</v>
@@ -3243,10 +3291,10 @@
         <v>44953</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3254,7 +3302,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5">
         <v>899</v>
@@ -3263,10 +3311,10 @@
         <v>44953</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3274,7 +3322,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5">
         <v>927</v>
@@ -3283,10 +3331,10 @@
         <v>44953</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3294,7 +3342,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="C10" s="5">
         <v>764</v>
@@ -3303,10 +3351,10 @@
         <v>44953</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3314,7 +3362,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5">
         <v>801</v>
@@ -3323,10 +3371,10 @@
         <v>44953</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3334,7 +3382,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5">
         <v>871</v>
@@ -3343,10 +3391,10 @@
         <v>44953</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3354,7 +3402,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C13" s="5">
         <v>962</v>
@@ -3363,10 +3411,10 @@
         <v>44953</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3374,7 +3422,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C14" s="5">
         <v>817</v>
@@ -3383,10 +3431,10 @@
         <v>44953</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3394,7 +3442,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5">
         <v>752</v>
@@ -3403,10 +3451,10 @@
         <v>44953</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3414,7 +3462,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C16" s="5">
         <v>988</v>
@@ -3423,10 +3471,10 @@
         <v>44953</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3434,7 +3482,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="C17" s="5">
         <v>890</v>
@@ -3443,10 +3491,10 @@
         <v>44953</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3454,7 +3502,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C18" s="5">
         <v>784</v>
@@ -3463,10 +3511,10 @@
         <v>44953</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3474,7 +3522,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C19" s="5">
         <v>943</v>
@@ -3483,10 +3531,10 @@
         <v>44953</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3494,7 +3542,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="C20" s="5">
         <v>975</v>
@@ -3503,10 +3551,10 @@
         <v>44953</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -3514,7 +3562,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
       <c r="C21" s="5">
         <v>826</v>
@@ -3523,10 +3571,10 @@
         <v>44953</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3534,7 +3582,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="C22" s="5">
         <v>902</v>
@@ -3543,10 +3591,10 @@
         <v>44953</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3554,7 +3602,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="C23" s="5">
         <v>769</v>
@@ -3563,10 +3611,10 @@
         <v>44953</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3574,7 +3622,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="C24" s="5">
         <v>810</v>
@@ -3583,10 +3631,10 @@
         <v>44953</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3594,7 +3642,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="C25" s="5">
         <v>976</v>
@@ -3603,10 +3651,10 @@
         <v>44953</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3614,7 +3662,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="C26" s="5">
         <v>955</v>
@@ -3623,10 +3671,10 @@
         <v>44953</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3634,7 +3682,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="C27" s="5">
         <v>791</v>
@@ -3643,10 +3691,10 @@
         <v>44953</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3654,7 +3702,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C28" s="5">
         <v>937</v>
@@ -3663,10 +3711,10 @@
         <v>44953</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3674,7 +3722,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>3</v>
+        <v>127</v>
       </c>
       <c r="C29" s="5">
         <v>899</v>
@@ -3683,10 +3731,10 @@
         <v>44953</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3694,7 +3742,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="C30" s="5">
         <v>768</v>
@@ -3703,10 +3751,10 @@
         <v>44953</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3714,7 +3762,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="C31" s="7">
         <v>834</v>
@@ -3723,10 +3771,10 @@
         <v>44953</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3744,7 +3792,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C31"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3763,36 +3811,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="D2" s="14">
         <v>44981</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3800,7 +3848,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5">
         <v>967</v>
@@ -3809,10 +3857,10 @@
         <v>44981</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3820,7 +3868,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5">
         <v>754</v>
@@ -3829,10 +3877,10 @@
         <v>44981</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3840,7 +3888,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="C5" s="5">
         <v>893</v>
@@ -3849,10 +3897,10 @@
         <v>44981</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3860,7 +3908,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5">
         <v>817</v>
@@ -3869,10 +3917,10 @@
         <v>44981</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3880,7 +3928,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="C7" s="5">
         <v>981</v>
@@ -3889,10 +3937,10 @@
         <v>44981</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3900,7 +3948,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5">
         <v>770</v>
@@ -3909,10 +3957,10 @@
         <v>44981</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3920,7 +3968,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5">
         <v>868</v>
@@ -3929,10 +3977,10 @@
         <v>44981</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3940,7 +3988,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="C10" s="5">
         <v>799</v>
@@ -3949,10 +3997,10 @@
         <v>44981</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3960,7 +4008,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5">
         <v>945</v>
@@ -3969,10 +4017,10 @@
         <v>44981</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3980,7 +4028,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5">
         <v>764</v>
@@ -3989,10 +4037,10 @@
         <v>44981</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4000,7 +4048,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C13" s="5">
         <v>956</v>
@@ -4009,10 +4057,10 @@
         <v>44981</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4020,7 +4068,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C14" s="5">
         <v>791</v>
@@ -4029,10 +4077,10 @@
         <v>44981</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4040,7 +4088,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5">
         <v>823</v>
@@ -4049,10 +4097,10 @@
         <v>44981</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -4060,7 +4108,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C16" s="5">
         <v>982</v>
@@ -4069,10 +4117,10 @@
         <v>44981</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4080,7 +4128,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="C17" s="5">
         <v>871</v>
@@ -4089,10 +4137,10 @@
         <v>44981</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4100,7 +4148,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C18" s="5">
         <v>898</v>
@@ -4109,10 +4157,10 @@
         <v>44981</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4120,7 +4168,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C19" s="5">
         <v>938</v>
@@ -4129,10 +4177,10 @@
         <v>44981</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4140,7 +4188,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="C20" s="5">
         <v>789</v>
@@ -4149,10 +4197,10 @@
         <v>44981</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4160,7 +4208,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
       <c r="C21" s="5">
         <v>903</v>
@@ -4169,10 +4217,10 @@
         <v>44981</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4180,7 +4228,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="C22" s="5">
         <v>785</v>
@@ -4189,10 +4237,10 @@
         <v>44981</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4200,7 +4248,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="C23" s="5">
         <v>972</v>
@@ -4209,10 +4257,10 @@
         <v>44981</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4220,7 +4268,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="C24" s="5">
         <v>752</v>
@@ -4229,10 +4277,10 @@
         <v>44981</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4240,7 +4288,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="C25" s="5">
         <v>965</v>
@@ -4249,10 +4297,10 @@
         <v>44981</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4260,7 +4308,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="C26" s="5">
         <v>809</v>
@@ -4269,10 +4317,10 @@
         <v>44981</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4280,7 +4328,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="C27" s="5">
         <v>920</v>
@@ -4289,10 +4337,10 @@
         <v>44981</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4300,7 +4348,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C28" s="5">
         <v>785</v>
@@ -4309,10 +4357,10 @@
         <v>44981</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4320,7 +4368,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>3</v>
+        <v>127</v>
       </c>
       <c r="C29" s="5">
         <v>952</v>
@@ -4329,10 +4377,10 @@
         <v>44981</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4340,7 +4388,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="C30" s="5">
         <v>976</v>
@@ -4349,10 +4397,10 @@
         <v>44981</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4360,7 +4408,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="C31" s="7">
         <v>793</v>
@@ -4369,10 +4417,10 @@
         <v>44981</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -4389,7 +4437,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C2:C31"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4408,36 +4456,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>862</v>
+        <v>800</v>
       </c>
       <c r="D2" s="14">
         <v>45016</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4445,7 +4493,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5">
         <v>787</v>
@@ -4454,10 +4502,10 @@
         <v>45016</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4465,7 +4513,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5">
         <v>925</v>
@@ -4474,10 +4522,10 @@
         <v>45016</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4485,7 +4533,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="C5" s="5">
         <v>978</v>
@@ -4494,10 +4542,10 @@
         <v>45016</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4505,7 +4553,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5">
         <v>801</v>
@@ -4514,10 +4562,10 @@
         <v>45016</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4525,7 +4573,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="C7" s="5">
         <v>954</v>
@@ -4534,10 +4582,10 @@
         <v>45016</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4545,7 +4593,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5">
         <v>769</v>
@@ -4554,10 +4602,10 @@
         <v>45016</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4565,7 +4613,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5">
         <v>840</v>
@@ -4574,10 +4622,10 @@
         <v>45016</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4585,7 +4633,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="C10" s="5">
         <v>892</v>
@@ -4594,10 +4642,10 @@
         <v>45016</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4605,7 +4653,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5">
         <v>759</v>
@@ -4614,10 +4662,10 @@
         <v>45016</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4625,7 +4673,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5">
         <v>983</v>
@@ -4634,10 +4682,10 @@
         <v>45016</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4645,7 +4693,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C13" s="5">
         <v>872</v>
@@ -4654,10 +4702,10 @@
         <v>45016</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4665,7 +4713,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C14" s="5">
         <v>937</v>
@@ -4674,10 +4722,10 @@
         <v>45016</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4685,7 +4733,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5">
         <v>794</v>
@@ -4694,10 +4742,10 @@
         <v>45016</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -4705,7 +4753,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C16" s="5">
         <v>968</v>
@@ -4714,10 +4762,10 @@
         <v>45016</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4725,7 +4773,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="C17" s="5">
         <v>783</v>
@@ -4734,10 +4782,10 @@
         <v>45016</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4745,7 +4793,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C18" s="5">
         <v>965</v>
@@ -4754,10 +4802,10 @@
         <v>45016</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4765,7 +4813,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C19" s="5">
         <v>812</v>
@@ -4774,10 +4822,10 @@
         <v>45016</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4785,7 +4833,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="C20" s="5">
         <v>911</v>
@@ -4794,10 +4842,10 @@
         <v>45016</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4805,7 +4853,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
       <c r="C21" s="5">
         <v>758</v>
@@ -4814,10 +4862,10 @@
         <v>45016</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4825,7 +4873,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="C22" s="5">
         <v>991</v>
@@ -4834,10 +4882,10 @@
         <v>45016</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4845,7 +4893,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="C23" s="5">
         <v>902</v>
@@ -4854,10 +4902,10 @@
         <v>45016</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4865,7 +4913,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="C24" s="5">
         <v>782</v>
@@ -4874,10 +4922,10 @@
         <v>45016</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4885,7 +4933,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="C25" s="5">
         <v>959</v>
@@ -4894,10 +4942,10 @@
         <v>45016</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4905,7 +4953,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="C26" s="5">
         <v>827</v>
@@ -4914,10 +4962,10 @@
         <v>45016</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4925,7 +4973,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="C27" s="5">
         <v>903</v>
@@ -4934,10 +4982,10 @@
         <v>45016</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4945,7 +4993,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C28" s="5">
         <v>773</v>
@@ -4954,10 +5002,10 @@
         <v>45016</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4965,7 +5013,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>3</v>
+        <v>127</v>
       </c>
       <c r="C29" s="5">
         <v>898</v>
@@ -4974,10 +5022,10 @@
         <v>45016</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4985,7 +5033,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="C30" s="5">
         <v>965</v>
@@ -4994,10 +5042,10 @@
         <v>45016</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -5005,7 +5053,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="C31" s="7">
         <v>789</v>
@@ -5014,10 +5062,10 @@
         <v>45016</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -5034,7 +5082,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C31"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5053,36 +5101,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>972</v>
+        <v>800</v>
       </c>
       <c r="D2" s="14">
         <v>45044</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5090,7 +5138,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5">
         <v>794</v>
@@ -5099,10 +5147,10 @@
         <v>45044</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5110,7 +5158,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5">
         <v>812</v>
@@ -5119,10 +5167,10 @@
         <v>45044</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -5130,7 +5178,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="C5" s="5">
         <v>965</v>
@@ -5139,10 +5187,10 @@
         <v>45044</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -5150,7 +5198,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5">
         <v>889</v>
@@ -5159,10 +5207,10 @@
         <v>45044</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5170,7 +5218,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="C7" s="5">
         <v>769</v>
@@ -5179,10 +5227,10 @@
         <v>45044</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -5190,7 +5238,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5">
         <v>825</v>
@@ -5199,10 +5247,10 @@
         <v>45044</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -5210,7 +5258,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5">
         <v>782</v>
@@ -5219,10 +5267,10 @@
         <v>45044</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -5230,7 +5278,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="C10" s="5">
         <v>938</v>
@@ -5239,10 +5287,10 @@
         <v>45044</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -5250,7 +5298,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5">
         <v>851</v>
@@ -5259,10 +5307,10 @@
         <v>45044</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -5270,7 +5318,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5">
         <v>797</v>
@@ -5279,10 +5327,10 @@
         <v>45044</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -5290,7 +5338,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C13" s="5">
         <v>902</v>
@@ -5299,10 +5347,10 @@
         <v>45044</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -5310,7 +5358,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C14" s="5">
         <v>763</v>
@@ -5319,10 +5367,10 @@
         <v>45044</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -5330,7 +5378,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5">
         <v>983</v>
@@ -5339,10 +5387,10 @@
         <v>45044</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -5350,7 +5398,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C16" s="5">
         <v>860</v>
@@ -5359,10 +5407,10 @@
         <v>45044</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -5370,7 +5418,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="C17" s="5">
         <v>775</v>
@@ -5379,10 +5427,10 @@
         <v>45044</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -5390,7 +5438,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C18" s="5">
         <v>956</v>
@@ -5399,10 +5447,10 @@
         <v>45044</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -5410,7 +5458,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C19" s="5">
         <v>791</v>
@@ -5419,10 +5467,10 @@
         <v>45044</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -5430,7 +5478,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="C20" s="5">
         <v>872</v>
@@ -5439,10 +5487,10 @@
         <v>45044</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -5450,7 +5498,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
       <c r="C21" s="5">
         <v>928</v>
@@ -5459,10 +5507,10 @@
         <v>45044</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -5470,7 +5518,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="C22" s="5">
         <v>810</v>
@@ -5479,10 +5527,10 @@
         <v>45044</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -5490,7 +5538,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="C23" s="5">
         <v>759</v>
@@ -5499,10 +5547,10 @@
         <v>45044</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -5510,7 +5558,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="C24" s="5">
         <v>967</v>
@@ -5519,10 +5567,10 @@
         <v>45044</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -5530,7 +5578,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="C25" s="5">
         <v>925</v>
@@ -5539,10 +5587,10 @@
         <v>45044</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -5550,7 +5598,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="C26" s="5">
         <v>788</v>
@@ -5559,10 +5607,10 @@
         <v>45044</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -5570,7 +5618,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="C27" s="5">
         <v>942</v>
@@ -5579,10 +5627,10 @@
         <v>45044</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -5590,7 +5638,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C28" s="5">
         <v>869</v>
@@ -5599,10 +5647,10 @@
         <v>45044</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -5610,7 +5658,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>3</v>
+        <v>127</v>
       </c>
       <c r="C29" s="5">
         <v>976</v>
@@ -5619,10 +5667,10 @@
         <v>45044</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -5630,7 +5678,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="C30" s="5">
         <v>791</v>
@@ -5639,10 +5687,10 @@
         <v>45044</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -5650,7 +5698,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="C31" s="7">
         <v>832</v>
@@ -5659,10 +5707,10 @@
         <v>45044</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -5679,7 +5727,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5698,36 +5746,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>893</v>
+        <v>800</v>
       </c>
       <c r="D2" s="14">
         <v>45072</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5735,7 +5783,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5">
         <v>817</v>
@@ -5744,10 +5792,10 @@
         <v>45072</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5755,7 +5803,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5">
         <v>964</v>
@@ -5764,10 +5812,10 @@
         <v>45072</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -5775,7 +5823,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="C5" s="5">
         <v>782</v>
@@ -5784,10 +5832,10 @@
         <v>45072</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -5795,7 +5843,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5">
         <v>926</v>
@@ -5804,10 +5852,10 @@
         <v>45072</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5815,7 +5863,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="C7" s="5">
         <v>798</v>
@@ -5824,10 +5872,10 @@
         <v>45072</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -5835,7 +5883,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5">
         <v>952</v>
@@ -5844,10 +5892,10 @@
         <v>45072</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -5855,7 +5903,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5">
         <v>867</v>
@@ -5864,10 +5912,10 @@
         <v>45072</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -5875,7 +5923,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="C10" s="5">
         <v>791</v>
@@ -5884,10 +5932,10 @@
         <v>45072</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -5895,7 +5943,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5">
         <v>811</v>
@@ -5904,10 +5952,10 @@
         <v>45072</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -5915,7 +5963,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5">
         <v>975</v>
@@ -5924,10 +5972,10 @@
         <v>45072</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -5935,7 +5983,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C13" s="5">
         <v>757</v>
@@ -5944,10 +5992,10 @@
         <v>45072</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -5955,7 +6003,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C14" s="5">
         <v>938</v>
@@ -5964,10 +6012,10 @@
         <v>45072</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -5975,7 +6023,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5">
         <v>859</v>
@@ -5984,10 +6032,10 @@
         <v>45072</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -5995,7 +6043,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C16" s="5">
         <v>790</v>
@@ -6004,10 +6052,10 @@
         <v>45072</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -6015,7 +6063,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="C17" s="5">
         <v>928</v>
@@ -6024,10 +6072,10 @@
         <v>45072</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -6035,7 +6083,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C18" s="5">
         <v>805</v>
@@ -6044,10 +6092,10 @@
         <v>45072</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -6055,7 +6103,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C19" s="5">
         <v>863</v>
@@ -6064,10 +6112,10 @@
         <v>45072</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -6075,7 +6123,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="C20" s="5">
         <v>786</v>
@@ -6084,10 +6132,10 @@
         <v>45072</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -6095,7 +6143,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
       <c r="C21" s="5">
         <v>976</v>
@@ -6104,10 +6152,10 @@
         <v>45072</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -6115,7 +6163,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="C22" s="5">
         <v>899</v>
@@ -6124,10 +6172,10 @@
         <v>45072</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -6135,7 +6183,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="C23" s="5">
         <v>764</v>
@@ -6144,10 +6192,10 @@
         <v>45072</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -6155,7 +6203,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="C24" s="5">
         <v>931</v>
@@ -6164,10 +6212,10 @@
         <v>45072</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L24" s="18"/>
     </row>
@@ -6176,7 +6224,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="C25" s="5">
         <v>843</v>
@@ -6185,10 +6233,10 @@
         <v>45072</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -6196,7 +6244,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="C26" s="5">
         <v>972</v>
@@ -6205,10 +6253,10 @@
         <v>45072</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -6216,7 +6264,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="C27" s="5">
         <v>816</v>
@@ -6225,10 +6273,10 @@
         <v>45072</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -6236,7 +6284,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C28" s="5">
         <v>756</v>
@@ -6245,10 +6293,10 @@
         <v>45072</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -6256,7 +6304,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>3</v>
+        <v>127</v>
       </c>
       <c r="C29" s="5">
         <v>915</v>
@@ -6265,10 +6313,10 @@
         <v>45072</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -6276,7 +6324,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="C30" s="5">
         <v>783</v>
@@ -6285,10 +6333,10 @@
         <v>45072</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -6296,7 +6344,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="C31" s="7">
         <v>894</v>
@@ -6305,10 +6353,10 @@
         <v>45072</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>